<commit_message>
Unit Test Filter Search
</commit_message>
<xml_diff>
--- a/TestData/Data/Former.xlsx
+++ b/TestData/Data/Former.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fouad.Systems\Desktop\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Trainning_Institution_System\1-Cplus\TestData\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="108">
   <si>
     <t>03/09/2018 10:59:28</t>
   </si>
@@ -38,9 +38,6 @@
     <t>formateur8@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_8</t>
-  </si>
-  <si>
     <t>Vide</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>Matricule_8</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>formateur7@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_7</t>
-  </si>
-  <si>
     <t>17/08/2018 00:00:06</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>Nom7</t>
   </si>
   <si>
-    <t>Matricule_7</t>
-  </si>
-  <si>
     <t>28</t>
   </si>
   <si>
@@ -113,9 +101,6 @@
     <t>formateur6@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_6</t>
-  </si>
-  <si>
     <t>17/08/2018 00:00:05</t>
   </si>
   <si>
@@ -125,9 +110,6 @@
     <t>Nom6</t>
   </si>
   <si>
-    <t>Matricule_6</t>
-  </si>
-  <si>
     <t>ANGLAIS</t>
   </si>
   <si>
@@ -137,9 +119,6 @@
     <t>formateur5@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_5</t>
-  </si>
-  <si>
     <t>17/08/2018 00:00:04</t>
   </si>
   <si>
@@ -149,9 +128,6 @@
     <t>Nom5</t>
   </si>
   <si>
-    <t>Matricule_5</t>
-  </si>
-  <si>
     <t>ARABE</t>
   </si>
   <si>
@@ -161,9 +137,6 @@
     <t>formateur4@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_4</t>
-  </si>
-  <si>
     <t>17/08/2018 00:00:03</t>
   </si>
   <si>
@@ -173,9 +146,6 @@
     <t>Nom4</t>
   </si>
   <si>
-    <t>Matricule_4</t>
-  </si>
-  <si>
     <t>Français</t>
   </si>
   <si>
@@ -185,9 +155,6 @@
     <t>formateur3@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_3</t>
-  </si>
-  <si>
     <t>17/08/2018 00:00:02</t>
   </si>
   <si>
@@ -197,9 +164,6 @@
     <t>Nom3</t>
   </si>
   <si>
-    <t>Matricule_3</t>
-  </si>
-  <si>
     <t>DEVELOPPEMENT</t>
   </si>
   <si>
@@ -209,9 +173,6 @@
     <t>formateur2@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_2</t>
-  </si>
-  <si>
     <t>17/08/2018 00:00:01</t>
   </si>
   <si>
@@ -221,9 +182,6 @@
     <t>Nom2</t>
   </si>
   <si>
-    <t>Matricule_2</t>
-  </si>
-  <si>
     <t>INFOGRAPHIE</t>
   </si>
   <si>
@@ -236,9 +194,6 @@
     <t>formateur1@ofppt.ma</t>
   </si>
   <si>
-    <t>CIN_1</t>
-  </si>
-  <si>
     <t>17/08/2018 00:00:00</t>
   </si>
   <si>
@@ -248,9 +203,6 @@
     <t>Nom1</t>
   </si>
   <si>
-    <t>Matricule_1</t>
-  </si>
-  <si>
     <t>RESEAU</t>
   </si>
   <si>
@@ -324,6 +276,78 @@
   </si>
   <si>
     <t>Specialité du formateur</t>
+  </si>
+  <si>
+    <t>Nom_Formateur1</t>
+  </si>
+  <si>
+    <t>Nom_Formateur2</t>
+  </si>
+  <si>
+    <t>Nom_Formateur3</t>
+  </si>
+  <si>
+    <t>Nom_Formateur4</t>
+  </si>
+  <si>
+    <t>Nom_Formateur5</t>
+  </si>
+  <si>
+    <t>Nom_Formateur6</t>
+  </si>
+  <si>
+    <t>Nom_Formateur7</t>
+  </si>
+  <si>
+    <t>Nom_Formateur8</t>
+  </si>
+  <si>
+    <t>Matricule_t_2</t>
+  </si>
+  <si>
+    <t>Matricule_t_1</t>
+  </si>
+  <si>
+    <t>Matricule_t_3</t>
+  </si>
+  <si>
+    <t>Matricule_t_4</t>
+  </si>
+  <si>
+    <t>Matricule_t_5</t>
+  </si>
+  <si>
+    <t>Matricule_t_6</t>
+  </si>
+  <si>
+    <t>Matricule_t_7</t>
+  </si>
+  <si>
+    <t>Matricule_t_8</t>
+  </si>
+  <si>
+    <t>CIN_t_1</t>
+  </si>
+  <si>
+    <t>CIN_t_2</t>
+  </si>
+  <si>
+    <t>CIN_t_3</t>
+  </si>
+  <si>
+    <t>CIN_t_4</t>
+  </si>
+  <si>
+    <t>CIN_t_5</t>
+  </si>
+  <si>
+    <t>CIN_t_6</t>
+  </si>
+  <si>
+    <t>CIN_t_7</t>
+  </si>
+  <si>
+    <t>CIN_t_8</t>
   </si>
 </sst>
 </file>
@@ -686,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +722,7 @@
     <col min="4" max="4" width="30.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="35" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" style="1" customWidth="1"/>
@@ -719,503 +743,503 @@
     <col min="25" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="V2" s="1">
         <v>1</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="V3" s="1">
         <v>2</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="V4" s="1">
         <v>3</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="X4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="V5" s="1">
         <v>4</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="X5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="V6" s="1">
         <v>5</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="X6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="V7" s="1">
         <v>6</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="X7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="V8" s="1">
         <v>7</v>
@@ -1227,51 +1251,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>4</v>
+        <v>107</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>

</xml_diff>